<commit_message>
show holidays on chart
</commit_message>
<xml_diff>
--- a/test_gantt_chart.xlsx
+++ b/test_gantt_chart.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Project Info" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Work Schedules" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Holiday Schedule" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -34,7 +36,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -51,6 +53,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC107"/>
+        <bgColor rgb="00FFC107"/>
       </patternFill>
     </fill>
   </fills>
@@ -72,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -83,9 +91,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -451,10 +473,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AU7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -464,13 +486,13 @@
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="3" customWidth="1" min="7" max="7"/>
-    <col width="3" customWidth="1" min="8" max="8"/>
-    <col width="3" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
     <col width="3" customWidth="1" min="10" max="10"/>
     <col width="3" customWidth="1" min="11" max="11"/>
     <col width="3" customWidth="1" min="12" max="12"/>
@@ -506,6 +528,9 @@
     <col width="3" customWidth="1" min="42" max="42"/>
     <col width="3" customWidth="1" min="43" max="43"/>
     <col width="3" customWidth="1" min="44" max="44"/>
+    <col width="3" customWidth="1" min="45" max="45"/>
+    <col width="3" customWidth="1" min="46" max="46"/>
+    <col width="3" customWidth="1" min="47" max="47"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -516,407 +541,422 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Depends On</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Assigned To</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Estimated Duration</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Availability (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Contingency (%)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Actual Duration</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Start Date</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>End Date</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>01/08</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>01/09</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>01/10</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>01/11</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>01/12</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>01/13</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="P1" s="2" t="inlineStr">
         <is>
           <t>01/14</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>01/15</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="R1" s="2" t="inlineStr">
         <is>
           <t>01/16</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="S1" s="2" t="inlineStr">
         <is>
           <t>01/17</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="T1" s="2" t="inlineStr">
         <is>
           <t>01/18</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="U1" s="2" t="inlineStr">
         <is>
           <t>01/19</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="V1" s="2" t="inlineStr">
         <is>
           <t>01/20</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="W1" s="2" t="inlineStr">
         <is>
           <t>01/21</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>01/22</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="Y1" s="2" t="inlineStr">
         <is>
           <t>01/23</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="Z1" s="2" t="inlineStr">
         <is>
           <t>01/24</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="AA1" s="2" t="inlineStr">
         <is>
           <t>01/25</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="AB1" s="2" t="inlineStr">
         <is>
           <t>01/26</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="AC1" s="2" t="inlineStr">
         <is>
           <t>01/27</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AD1" s="2" t="inlineStr">
         <is>
           <t>01/28</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AE1" s="2" t="inlineStr">
         <is>
           <t>01/29</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AF1" s="2" t="inlineStr">
         <is>
           <t>01/30</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AG1" s="2" t="inlineStr">
         <is>
           <t>01/31</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AH1" s="2" t="inlineStr">
         <is>
           <t>02/01</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AI1" s="2" t="inlineStr">
         <is>
           <t>02/02</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AJ1" s="2" t="inlineStr">
         <is>
           <t>02/03</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AK1" s="2" t="inlineStr">
         <is>
           <t>02/04</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AL1" s="2" t="inlineStr">
         <is>
           <t>02/05</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AM1" s="2" t="inlineStr">
         <is>
           <t>02/06</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AN1" s="2" t="inlineStr">
         <is>
           <t>02/07</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AO1" s="2" t="inlineStr">
         <is>
           <t>02/08</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AP1" s="2" t="inlineStr">
         <is>
           <t>02/09</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AQ1" s="2" t="inlineStr">
         <is>
           <t>02/10</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AR1" s="2" t="inlineStr">
         <is>
           <t>02/11</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AS1" s="2" t="inlineStr">
         <is>
           <t>02/12</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AT1" s="2" t="inlineStr">
         <is>
           <t>02/13</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AU1" s="2" t="inlineStr">
         <is>
           <t>02/14</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="G2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="R2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="S2" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="W2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="U2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="Y2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="Z2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="AB2" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AC2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AA2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AB2" s="1" t="inlineStr">
+      <c r="AE2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AF2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="AD2" s="1" t="inlineStr">
+      <c r="AG2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="AE2" s="1" t="inlineStr">
+      <c r="AH2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="AF2" s="1" t="inlineStr">
+      <c r="AI2" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="AG2" s="1" t="inlineStr">
+      <c r="AJ2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AH2" s="1" t="inlineStr">
+      <c r="AK2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AI2" s="1" t="inlineStr">
+      <c r="AL2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="AJ2" s="1" t="inlineStr">
+      <c r="AM2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="AK2" s="1" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="AL2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="AM2" s="1" t="inlineStr">
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="AN2" s="1" t="inlineStr">
+      <c r="AQ2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AO2" s="1" t="inlineStr">
+      <c r="AR2" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="AP2" s="1" t="inlineStr">
+      <c r="AS2" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="AQ2" s="1" t="inlineStr">
+      <c r="AT2" s="1" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="AR2" s="1" t="inlineStr">
+      <c r="AU2" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
@@ -928,65 +968,80 @@
           <t>Requirements Gathering</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>3</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>2024-01-08</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="I3" s="3" t="inlineStr">
         <is>
           <t>2024-01-11</t>
         </is>
       </c>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="4" t="n"/>
-      <c r="I3" s="5" t="n"/>
-      <c r="J3" s="4" t="n"/>
-      <c r="K3" s="5" t="n"/>
-      <c r="L3" s="5" t="n"/>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="5" t="n"/>
-      <c r="O3" s="5" t="n"/>
-      <c r="P3" s="5" t="n"/>
-      <c r="Q3" s="5" t="n"/>
-      <c r="R3" s="5" t="n"/>
-      <c r="S3" s="5" t="n"/>
-      <c r="T3" s="5" t="n"/>
-      <c r="U3" s="5" t="n"/>
-      <c r="V3" s="5" t="n"/>
-      <c r="W3" s="5" t="n"/>
-      <c r="X3" s="5" t="n"/>
-      <c r="Y3" s="5" t="n"/>
-      <c r="Z3" s="5" t="n"/>
-      <c r="AA3" s="5" t="n"/>
-      <c r="AB3" s="5" t="n"/>
-      <c r="AC3" s="5" t="n"/>
-      <c r="AD3" s="5" t="n"/>
-      <c r="AE3" s="5" t="n"/>
-      <c r="AF3" s="5" t="n"/>
-      <c r="AG3" s="5" t="n"/>
-      <c r="AH3" s="5" t="n"/>
-      <c r="AI3" s="5" t="n"/>
-      <c r="AJ3" s="5" t="n"/>
-      <c r="AK3" s="5" t="n"/>
-      <c r="AL3" s="5" t="n"/>
-      <c r="AM3" s="5" t="n"/>
-      <c r="AN3" s="5" t="n"/>
-      <c r="AO3" s="5" t="n"/>
-      <c r="AP3" s="5" t="n"/>
-      <c r="AQ3" s="5" t="n"/>
-      <c r="AR3" s="5" t="n"/>
+      <c r="J3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6" t="n"/>
+      <c r="O3" s="6" t="n"/>
+      <c r="P3" s="6" t="n"/>
+      <c r="Q3" s="6" t="n"/>
+      <c r="R3" s="6" t="n"/>
+      <c r="S3" s="6" t="n"/>
+      <c r="T3" s="6" t="n"/>
+      <c r="U3" s="6" t="n"/>
+      <c r="V3" s="6" t="n"/>
+      <c r="W3" s="6" t="n"/>
+      <c r="X3" s="6" t="n"/>
+      <c r="Y3" s="6" t="n"/>
+      <c r="Z3" s="6" t="n"/>
+      <c r="AA3" s="6" t="n"/>
+      <c r="AB3" s="6" t="n"/>
+      <c r="AC3" s="6" t="n"/>
+      <c r="AD3" s="6" t="n"/>
+      <c r="AE3" s="6" t="n"/>
+      <c r="AF3" s="6" t="n"/>
+      <c r="AG3" s="6" t="n"/>
+      <c r="AH3" s="6" t="n"/>
+      <c r="AI3" s="6" t="n"/>
+      <c r="AJ3" s="6" t="n"/>
+      <c r="AK3" s="6" t="n"/>
+      <c r="AL3" s="6" t="n"/>
+      <c r="AM3" s="6" t="n"/>
+      <c r="AN3" s="6" t="n"/>
+      <c r="AO3" s="6" t="n"/>
+      <c r="AP3" s="6" t="n"/>
+      <c r="AQ3" s="6" t="n"/>
+      <c r="AR3" s="6" t="n"/>
+      <c r="AS3" s="6" t="n"/>
+      <c r="AT3" s="6" t="n"/>
+      <c r="AU3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -996,63 +1051,88 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
+          <t>Requirements Gathering</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
           <t>Bob</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="D4" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="E4" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t>2024-01-12</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
         <is>
           <t>2024-01-22</t>
         </is>
       </c>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="5" t="n"/>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="5" t="n"/>
-      <c r="K4" s="4" t="n"/>
-      <c r="L4" s="5" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="4" t="n"/>
-      <c r="P4" s="4" t="n"/>
-      <c r="Q4" s="4" t="n"/>
-      <c r="R4" s="4" t="n"/>
-      <c r="S4" s="5" t="n"/>
-      <c r="T4" s="5" t="n"/>
-      <c r="U4" s="4" t="n"/>
-      <c r="V4" s="5" t="n"/>
-      <c r="W4" s="5" t="n"/>
-      <c r="X4" s="5" t="n"/>
-      <c r="Y4" s="5" t="n"/>
-      <c r="Z4" s="5" t="n"/>
-      <c r="AA4" s="5" t="n"/>
-      <c r="AB4" s="5" t="n"/>
-      <c r="AC4" s="5" t="n"/>
-      <c r="AD4" s="5" t="n"/>
-      <c r="AE4" s="5" t="n"/>
-      <c r="AF4" s="5" t="n"/>
-      <c r="AG4" s="5" t="n"/>
-      <c r="AH4" s="5" t="n"/>
-      <c r="AI4" s="5" t="n"/>
-      <c r="AJ4" s="5" t="n"/>
-      <c r="AK4" s="5" t="n"/>
-      <c r="AL4" s="5" t="n"/>
-      <c r="AM4" s="5" t="n"/>
-      <c r="AN4" s="5" t="n"/>
-      <c r="AO4" s="5" t="n"/>
-      <c r="AP4" s="5" t="n"/>
-      <c r="AQ4" s="5" t="n"/>
-      <c r="AR4" s="5" t="n"/>
+      <c r="J4" s="6" t="n"/>
+      <c r="K4" s="6" t="n"/>
+      <c r="L4" s="6" t="n"/>
+      <c r="M4" s="6" t="n"/>
+      <c r="N4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="n"/>
+      <c r="P4" s="6" t="n"/>
+      <c r="Q4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="6" t="n"/>
+      <c r="W4" s="6" t="n"/>
+      <c r="X4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="6" t="n"/>
+      <c r="Z4" s="6" t="n"/>
+      <c r="AA4" s="6" t="n"/>
+      <c r="AB4" s="6" t="n"/>
+      <c r="AC4" s="6" t="n"/>
+      <c r="AD4" s="6" t="n"/>
+      <c r="AE4" s="6" t="n"/>
+      <c r="AF4" s="6" t="n"/>
+      <c r="AG4" s="6" t="n"/>
+      <c r="AH4" s="6" t="n"/>
+      <c r="AI4" s="6" t="n"/>
+      <c r="AJ4" s="6" t="n"/>
+      <c r="AK4" s="6" t="n"/>
+      <c r="AL4" s="6" t="n"/>
+      <c r="AM4" s="6" t="n"/>
+      <c r="AN4" s="6" t="n"/>
+      <c r="AO4" s="6" t="n"/>
+      <c r="AP4" s="6" t="n"/>
+      <c r="AQ4" s="6" t="n"/>
+      <c r="AR4" s="6" t="n"/>
+      <c r="AS4" s="6" t="n"/>
+      <c r="AT4" s="6" t="n"/>
+      <c r="AU4" s="6" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -1062,63 +1142,98 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
+          <t>Design Mockups</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="D5" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="E5" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>2024-01-23</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>2024-02-07</t>
         </is>
       </c>
-      <c r="G5" s="5" t="n"/>
-      <c r="H5" s="5" t="n"/>
-      <c r="I5" s="5" t="n"/>
-      <c r="J5" s="5" t="n"/>
-      <c r="K5" s="5" t="n"/>
-      <c r="L5" s="5" t="n"/>
-      <c r="M5" s="5" t="n"/>
-      <c r="N5" s="5" t="n"/>
-      <c r="O5" s="5" t="n"/>
-      <c r="P5" s="5" t="n"/>
-      <c r="Q5" s="5" t="n"/>
-      <c r="R5" s="5" t="n"/>
-      <c r="S5" s="5" t="n"/>
-      <c r="T5" s="5" t="n"/>
-      <c r="U5" s="5" t="n"/>
-      <c r="V5" s="4" t="n"/>
-      <c r="W5" s="4" t="n"/>
-      <c r="X5" s="4" t="n"/>
-      <c r="Y5" s="4" t="n"/>
-      <c r="Z5" s="5" t="n"/>
-      <c r="AA5" s="5" t="n"/>
-      <c r="AB5" s="4" t="n"/>
-      <c r="AC5" s="4" t="n"/>
-      <c r="AD5" s="4" t="n"/>
-      <c r="AE5" s="4" t="n"/>
-      <c r="AF5" s="4" t="n"/>
-      <c r="AG5" s="5" t="n"/>
-      <c r="AH5" s="5" t="n"/>
-      <c r="AI5" s="4" t="n"/>
-      <c r="AJ5" s="4" t="n"/>
-      <c r="AK5" s="4" t="n"/>
-      <c r="AL5" s="5" t="n"/>
-      <c r="AM5" s="5" t="n"/>
-      <c r="AN5" s="5" t="n"/>
-      <c r="AO5" s="5" t="n"/>
-      <c r="AP5" s="5" t="n"/>
-      <c r="AQ5" s="5" t="n"/>
-      <c r="AR5" s="5" t="n"/>
+      <c r="J5" s="6" t="n"/>
+      <c r="K5" s="6" t="n"/>
+      <c r="L5" s="6" t="n"/>
+      <c r="M5" s="6" t="n"/>
+      <c r="N5" s="6" t="n"/>
+      <c r="O5" s="6" t="n"/>
+      <c r="P5" s="6" t="n"/>
+      <c r="Q5" s="6" t="n"/>
+      <c r="R5" s="6" t="n"/>
+      <c r="S5" s="6" t="n"/>
+      <c r="T5" s="6" t="n"/>
+      <c r="U5" s="6" t="n"/>
+      <c r="V5" s="6" t="n"/>
+      <c r="W5" s="6" t="n"/>
+      <c r="X5" s="6" t="n"/>
+      <c r="Y5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="6" t="n"/>
+      <c r="AD5" s="6" t="n"/>
+      <c r="AE5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="6" t="n"/>
+      <c r="AK5" s="6" t="n"/>
+      <c r="AL5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="6" t="n"/>
+      <c r="AP5" s="6" t="n"/>
+      <c r="AQ5" s="6" t="n"/>
+      <c r="AR5" s="6" t="n"/>
+      <c r="AS5" s="6" t="n"/>
+      <c r="AT5" s="6" t="n"/>
+      <c r="AU5" s="6" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -1128,63 +1243,92 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
+          <t>Design Mockups</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
           <t>Bob</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="D6" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="E6" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="H6" s="3" t="inlineStr">
         <is>
           <t>2024-01-23</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
         <is>
           <t>2024-02-02</t>
         </is>
       </c>
-      <c r="G6" s="5" t="n"/>
-      <c r="H6" s="5" t="n"/>
-      <c r="I6" s="5" t="n"/>
-      <c r="J6" s="5" t="n"/>
-      <c r="K6" s="5" t="n"/>
-      <c r="L6" s="5" t="n"/>
-      <c r="M6" s="5" t="n"/>
-      <c r="N6" s="5" t="n"/>
-      <c r="O6" s="5" t="n"/>
-      <c r="P6" s="5" t="n"/>
-      <c r="Q6" s="5" t="n"/>
-      <c r="R6" s="5" t="n"/>
-      <c r="S6" s="5" t="n"/>
-      <c r="T6" s="5" t="n"/>
-      <c r="U6" s="5" t="n"/>
-      <c r="V6" s="4" t="n"/>
-      <c r="W6" s="4" t="n"/>
-      <c r="X6" s="4" t="n"/>
-      <c r="Y6" s="4" t="n"/>
-      <c r="Z6" s="5" t="n"/>
-      <c r="AA6" s="5" t="n"/>
-      <c r="AB6" s="4" t="n"/>
-      <c r="AC6" s="4" t="n"/>
-      <c r="AD6" s="4" t="n"/>
-      <c r="AE6" s="4" t="n"/>
-      <c r="AF6" s="4" t="n"/>
-      <c r="AG6" s="5" t="n"/>
-      <c r="AH6" s="5" t="n"/>
-      <c r="AI6" s="5" t="n"/>
-      <c r="AJ6" s="5" t="n"/>
-      <c r="AK6" s="5" t="n"/>
-      <c r="AL6" s="5" t="n"/>
-      <c r="AM6" s="5" t="n"/>
-      <c r="AN6" s="5" t="n"/>
-      <c r="AO6" s="5" t="n"/>
-      <c r="AP6" s="5" t="n"/>
-      <c r="AQ6" s="5" t="n"/>
-      <c r="AR6" s="5" t="n"/>
+      <c r="J6" s="6" t="n"/>
+      <c r="K6" s="6" t="n"/>
+      <c r="L6" s="6" t="n"/>
+      <c r="M6" s="6" t="n"/>
+      <c r="N6" s="6" t="n"/>
+      <c r="O6" s="6" t="n"/>
+      <c r="P6" s="6" t="n"/>
+      <c r="Q6" s="6" t="n"/>
+      <c r="R6" s="6" t="n"/>
+      <c r="S6" s="6" t="n"/>
+      <c r="T6" s="6" t="n"/>
+      <c r="U6" s="6" t="n"/>
+      <c r="V6" s="6" t="n"/>
+      <c r="W6" s="6" t="n"/>
+      <c r="X6" s="6" t="n"/>
+      <c r="Y6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="6" t="n"/>
+      <c r="AD6" s="6" t="n"/>
+      <c r="AE6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="6" t="n"/>
+      <c r="AK6" s="6" t="n"/>
+      <c r="AL6" s="6" t="n"/>
+      <c r="AM6" s="6" t="n"/>
+      <c r="AN6" s="6" t="n"/>
+      <c r="AO6" s="6" t="n"/>
+      <c r="AP6" s="6" t="n"/>
+      <c r="AQ6" s="6" t="n"/>
+      <c r="AR6" s="6" t="n"/>
+      <c r="AS6" s="6" t="n"/>
+      <c r="AT6" s="6" t="n"/>
+      <c r="AU6" s="6" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -1194,63 +1338,84 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
+          <t>Frontend Development</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
           <t>Alice</t>
         </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>5</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
         <is>
           <t>2024-02-08</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="I7" s="3" t="inlineStr">
         <is>
           <t>2024-02-14</t>
         </is>
       </c>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
-      <c r="I7" s="5" t="n"/>
-      <c r="J7" s="5" t="n"/>
-      <c r="K7" s="5" t="n"/>
-      <c r="L7" s="5" t="n"/>
-      <c r="M7" s="5" t="n"/>
-      <c r="N7" s="5" t="n"/>
-      <c r="O7" s="5" t="n"/>
-      <c r="P7" s="5" t="n"/>
-      <c r="Q7" s="5" t="n"/>
-      <c r="R7" s="5" t="n"/>
-      <c r="S7" s="5" t="n"/>
-      <c r="T7" s="5" t="n"/>
-      <c r="U7" s="5" t="n"/>
-      <c r="V7" s="5" t="n"/>
-      <c r="W7" s="5" t="n"/>
-      <c r="X7" s="5" t="n"/>
-      <c r="Y7" s="5" t="n"/>
-      <c r="Z7" s="5" t="n"/>
-      <c r="AA7" s="5" t="n"/>
-      <c r="AB7" s="5" t="n"/>
-      <c r="AC7" s="5" t="n"/>
-      <c r="AD7" s="5" t="n"/>
-      <c r="AE7" s="5" t="n"/>
-      <c r="AF7" s="5" t="n"/>
-      <c r="AG7" s="5" t="n"/>
-      <c r="AH7" s="5" t="n"/>
-      <c r="AI7" s="5" t="n"/>
-      <c r="AJ7" s="5" t="n"/>
-      <c r="AK7" s="5" t="n"/>
-      <c r="AL7" s="4" t="n"/>
-      <c r="AM7" s="4" t="n"/>
-      <c r="AN7" s="5" t="n"/>
-      <c r="AO7" s="5" t="n"/>
-      <c r="AP7" s="4" t="n"/>
-      <c r="AQ7" s="4" t="n"/>
-      <c r="AR7" s="4" t="n"/>
+      <c r="J7" s="6" t="n"/>
+      <c r="K7" s="6" t="n"/>
+      <c r="L7" s="6" t="n"/>
+      <c r="M7" s="6" t="n"/>
+      <c r="N7" s="6" t="n"/>
+      <c r="O7" s="6" t="n"/>
+      <c r="P7" s="6" t="n"/>
+      <c r="Q7" s="6" t="n"/>
+      <c r="R7" s="6" t="n"/>
+      <c r="S7" s="6" t="n"/>
+      <c r="T7" s="6" t="n"/>
+      <c r="U7" s="6" t="n"/>
+      <c r="V7" s="6" t="n"/>
+      <c r="W7" s="6" t="n"/>
+      <c r="X7" s="6" t="n"/>
+      <c r="Y7" s="6" t="n"/>
+      <c r="Z7" s="6" t="n"/>
+      <c r="AA7" s="6" t="n"/>
+      <c r="AB7" s="6" t="n"/>
+      <c r="AC7" s="6" t="n"/>
+      <c r="AD7" s="6" t="n"/>
+      <c r="AE7" s="6" t="n"/>
+      <c r="AF7" s="6" t="n"/>
+      <c r="AG7" s="6" t="n"/>
+      <c r="AH7" s="6" t="n"/>
+      <c r="AI7" s="6" t="n"/>
+      <c r="AJ7" s="6" t="n"/>
+      <c r="AK7" s="6" t="n"/>
+      <c r="AL7" s="6" t="n"/>
+      <c r="AM7" s="6" t="n"/>
+      <c r="AN7" s="6" t="n"/>
+      <c r="AO7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="6" t="n"/>
+      <c r="AR7" s="6" t="n"/>
+      <c r="AS7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1276,7 +1441,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Project Name:</t>
         </is>
@@ -1288,7 +1453,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>Start Date:</t>
         </is>
@@ -1300,7 +1465,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>End Date:</t>
         </is>
@@ -1312,13 +1477,223 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Total Duration (days):</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Employee Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C2" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="6" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Employee Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Holiday Dates</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>GLOBAL</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>